<commit_message>
Added v1.1.0 updated schematic. R3:1.5K->220R, R13,R14:470R->1.5K, rerouted UART1_, moved USB micro into board, placed resistors R14-to-R27 on front of PCB (no components on rear)
</commit_message>
<xml_diff>
--- a/Production Design Projects/ARM-mbed/mbedXdotShield/v1.1.0/mbedXdotShield-V_1_0_1-Europe-BOM.xlsx
+++ b/Production Design Projects/ARM-mbed/mbedXdotShield/v1.1.0/mbedXdotShield-V_1_0_1-Europe-BOM.xlsx
@@ -98,9 +98,6 @@
     <t>1.5K</t>
   </si>
   <si>
-    <t>R2, R3, R5, R8</t>
-  </si>
-  <si>
     <t>100nF</t>
   </si>
   <si>
@@ -152,9 +149,6 @@
     <t>220R</t>
   </si>
   <si>
-    <t>R14, R15, R16, R17, R18, R19, R20, R21, R22, R23, R24, R25, R26</t>
-  </si>
-  <si>
     <t>33R</t>
   </si>
   <si>
@@ -164,9 +158,6 @@
     <t>470R</t>
   </si>
   <si>
-    <t>R11, R12, R13</t>
-  </si>
-  <si>
     <t>47346-0001</t>
   </si>
   <si>
@@ -699,6 +690,15 @@
   </si>
   <si>
     <t>D1, D2, D3, D4, D5</t>
+  </si>
+  <si>
+    <t>R3, R14, R15, R16, R17, R18, R19, R20, R21, R22, R23, R24, R25, R26</t>
+  </si>
+  <si>
+    <t>R2, R5, R8, R12, R13</t>
+  </si>
+  <si>
+    <t>R11</t>
   </si>
 </sst>
 </file>
@@ -1135,7 +1135,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1201,22 +1201,22 @@
         <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G2" t="s">
+        <v>170</v>
+      </c>
+      <c r="H2" t="s">
+        <v>171</v>
+      </c>
+      <c r="I2" t="s">
+        <v>172</v>
+      </c>
+      <c r="J2" t="s">
         <v>173</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K2" t="s">
         <v>174</v>
-      </c>
-      <c r="I2" t="s">
-        <v>175</v>
-      </c>
-      <c r="J2" t="s">
-        <v>176</v>
-      </c>
-      <c r="K2" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1233,30 +1233,30 @@
         <v>402</v>
       </c>
       <c r="E3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F3" t="s">
         <v>15</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="K3" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
@@ -1268,22 +1268,22 @@
         <v>402</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>216</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>128</v>
       </c>
       <c r="K4" s="1">
         <v>2302656</v>
@@ -1291,34 +1291,34 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
         <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
       </c>
       <c r="D5">
         <v>402</v>
       </c>
       <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
         <v>20</v>
       </c>
-      <c r="F5" t="s">
-        <v>21</v>
-      </c>
       <c r="G5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="H5" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="I5" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="J5" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="K5">
         <v>1327666</v>
@@ -1326,34 +1326,34 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6">
         <v>603</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>136</v>
       </c>
       <c r="K6" s="1">
         <v>1327679</v>
@@ -1361,10 +1361,10 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
@@ -1373,57 +1373,57 @@
         <v>402</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F7" t="s">
         <v>15</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="H7" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="K7" t="s">
         <v>179</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="K7" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8">
         <v>603</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="K8" s="1">
         <v>1458902</v>
@@ -1431,77 +1431,77 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
         <v>28</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>29</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>30</v>
       </c>
-      <c r="E9" t="s">
-        <v>31</v>
-      </c>
       <c r="F9" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="G9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H9" t="s">
+        <v>164</v>
+      </c>
+      <c r="I9" t="s">
+        <v>165</v>
+      </c>
+      <c r="J9" t="s">
+        <v>166</v>
+      </c>
+      <c r="K9" t="s">
         <v>167</v>
-      </c>
-      <c r="I9" t="s">
-        <v>168</v>
-      </c>
-      <c r="J9" t="s">
-        <v>169</v>
-      </c>
-      <c r="K9" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10">
         <v>402</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G10" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="H10" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="I10" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="K10" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
@@ -1510,22 +1510,22 @@
         <v>402</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>215</v>
       </c>
       <c r="F11" t="s">
         <v>15</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="K11">
         <v>1514687</v>
@@ -1533,10 +1533,10 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
@@ -1545,33 +1545,33 @@
         <v>402</v>
       </c>
       <c r="E12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F12" t="s">
         <v>15</v>
       </c>
       <c r="G12" t="s">
+        <v>156</v>
+      </c>
+      <c r="H12" t="s">
+        <v>155</v>
+      </c>
+      <c r="I12" t="s">
+        <v>157</v>
+      </c>
+      <c r="J12" t="s">
+        <v>158</v>
+      </c>
+      <c r="K12" t="s">
         <v>159</v>
-      </c>
-      <c r="H12" t="s">
-        <v>158</v>
-      </c>
-      <c r="I12" t="s">
-        <v>160</v>
-      </c>
-      <c r="J12" t="s">
-        <v>161</v>
-      </c>
-      <c r="K12" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
@@ -1580,55 +1580,55 @@
         <v>402</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>217</v>
       </c>
       <c r="F13" t="s">
         <v>15</v>
       </c>
       <c r="G13" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="H13" t="s">
+        <v>160</v>
+      </c>
+      <c r="I13" t="s">
+        <v>161</v>
+      </c>
+      <c r="J13" t="s">
+        <v>162</v>
+      </c>
+      <c r="K13" t="s">
         <v>163</v>
-      </c>
-      <c r="I13" t="s">
-        <v>164</v>
-      </c>
-      <c r="J13" t="s">
-        <v>165</v>
-      </c>
-      <c r="K13" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" t="s">
         <v>40</v>
       </c>
-      <c r="C14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="G14" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E14" t="s">
-        <v>42</v>
-      </c>
-      <c r="F14" t="s">
-        <v>43</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="H14" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="K14" s="1">
         <v>1568026</v>
@@ -1636,69 +1636,69 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D15">
         <v>402</v>
       </c>
       <c r="E15" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="H15" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="K15" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D16">
         <v>402</v>
       </c>
       <c r="E16" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="K16" s="1">
         <v>2611902</v>
@@ -1706,34 +1706,34 @@
     </row>
     <row r="17" spans="1:11">
       <c r="A17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D17">
         <v>402</v>
       </c>
       <c r="E17" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G17" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="J17" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="K17" s="1">
         <v>2470460</v>
@@ -1741,69 +1741,69 @@
     </row>
     <row r="18" spans="1:11">
       <c r="A18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D18">
         <v>402</v>
       </c>
       <c r="E18" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="H18" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="K18" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="19" spans="1:11">
       <c r="A19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" t="s">
         <v>54</v>
       </c>
-      <c r="C19" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="G19" t="s">
         <v>55</v>
       </c>
-      <c r="E19" t="s">
+      <c r="H19" t="s">
+        <v>51</v>
+      </c>
+      <c r="I19" t="s">
         <v>56</v>
       </c>
-      <c r="F19" t="s">
+      <c r="J19" t="s">
         <v>57</v>
-      </c>
-      <c r="G19" t="s">
-        <v>58</v>
-      </c>
-      <c r="H19" t="s">
-        <v>54</v>
-      </c>
-      <c r="I19" t="s">
-        <v>59</v>
-      </c>
-      <c r="J19" t="s">
-        <v>60</v>
       </c>
       <c r="K19">
         <v>2414318</v>
@@ -1811,104 +1811,104 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" t="s">
+        <v>214</v>
+      </c>
+      <c r="F20" t="s">
+        <v>60</v>
+      </c>
+      <c r="G20" t="s">
         <v>61</v>
       </c>
-      <c r="C20" t="s">
-        <v>61</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="H20" t="s">
         <v>62</v>
       </c>
-      <c r="E20" t="s">
-        <v>217</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="I20" t="s">
         <v>63</v>
       </c>
-      <c r="G20" t="s">
+      <c r="J20" t="s">
         <v>64</v>
       </c>
-      <c r="H20" t="s">
+      <c r="K20" t="s">
         <v>65</v>
-      </c>
-      <c r="I20" t="s">
-        <v>66</v>
-      </c>
-      <c r="J20" t="s">
-        <v>67</v>
-      </c>
-      <c r="K20" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:11">
       <c r="A21">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B21" t="s">
+        <v>207</v>
+      </c>
+      <c r="C21" t="s">
+        <v>207</v>
+      </c>
+      <c r="D21" t="s">
+        <v>59</v>
+      </c>
+      <c r="E21" t="s">
+        <v>208</v>
+      </c>
+      <c r="F21" t="s">
+        <v>60</v>
+      </c>
+      <c r="G21" t="s">
+        <v>209</v>
+      </c>
+      <c r="H21" t="s">
         <v>210</v>
       </c>
-      <c r="C21" t="s">
-        <v>210</v>
-      </c>
-      <c r="D21" t="s">
-        <v>62</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="I21" t="s">
         <v>211</v>
       </c>
-      <c r="F21" t="s">
-        <v>63</v>
-      </c>
-      <c r="G21" t="s">
+      <c r="J21" t="s">
         <v>212</v>
       </c>
-      <c r="H21" t="s">
+      <c r="K21" t="s">
         <v>213</v>
-      </c>
-      <c r="I21" t="s">
-        <v>214</v>
-      </c>
-      <c r="J21" t="s">
-        <v>215</v>
-      </c>
-      <c r="K21" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="22" spans="1:11">
       <c r="A22">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" t="s">
         <v>69</v>
       </c>
-      <c r="C22" t="s">
-        <v>70</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="F22" t="s">
+        <v>186</v>
+      </c>
+      <c r="G22" t="s">
         <v>71</v>
       </c>
-      <c r="E22" t="s">
-        <v>72</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="H22" t="s">
+        <v>187</v>
+      </c>
+      <c r="I22" t="s">
+        <v>188</v>
+      </c>
+      <c r="J22" t="s">
         <v>189</v>
-      </c>
-      <c r="G22" t="s">
-        <v>74</v>
-      </c>
-      <c r="H22" t="s">
-        <v>190</v>
-      </c>
-      <c r="I22" t="s">
-        <v>191</v>
-      </c>
-      <c r="J22" t="s">
-        <v>192</v>
       </c>
       <c r="K22">
         <v>2322069</v>
@@ -1916,69 +1916,69 @@
     </row>
     <row r="23" spans="1:11">
       <c r="A23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23" t="s">
+        <v>77</v>
+      </c>
+      <c r="F23" t="s">
         <v>78</v>
       </c>
-      <c r="C23" t="s">
-        <v>78</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="G23" t="s">
         <v>79</v>
       </c>
-      <c r="E23" t="s">
+      <c r="H23" t="s">
+        <v>75</v>
+      </c>
+      <c r="I23" t="s">
         <v>80</v>
       </c>
-      <c r="F23" t="s">
+      <c r="J23" t="s">
         <v>81</v>
       </c>
-      <c r="G23" t="s">
+      <c r="K23" t="s">
         <v>82</v>
-      </c>
-      <c r="H23" t="s">
-        <v>78</v>
-      </c>
-      <c r="I23" t="s">
-        <v>83</v>
-      </c>
-      <c r="J23" t="s">
-        <v>84</v>
-      </c>
-      <c r="K23" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:11">
       <c r="A24">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D24" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" t="s">
+        <v>84</v>
+      </c>
+      <c r="F24" t="s">
+        <v>190</v>
+      </c>
+      <c r="G24" t="s">
         <v>71</v>
       </c>
-      <c r="E24" t="s">
-        <v>87</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="H24" t="s">
+        <v>191</v>
+      </c>
+      <c r="I24" t="s">
+        <v>192</v>
+      </c>
+      <c r="J24" t="s">
         <v>193</v>
-      </c>
-      <c r="G24" t="s">
-        <v>74</v>
-      </c>
-      <c r="H24" t="s">
-        <v>194</v>
-      </c>
-      <c r="I24" t="s">
-        <v>195</v>
-      </c>
-      <c r="J24" t="s">
-        <v>196</v>
       </c>
       <c r="K24">
         <v>2322070</v>
@@ -1986,118 +1986,118 @@
     </row>
     <row r="25" spans="1:11">
       <c r="A25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B25" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25" t="s">
+        <v>85</v>
+      </c>
+      <c r="D25" t="s">
+        <v>86</v>
+      </c>
+      <c r="E25" t="s">
+        <v>87</v>
+      </c>
+      <c r="F25" t="s">
         <v>88</v>
       </c>
-      <c r="C25" t="s">
-        <v>88</v>
-      </c>
-      <c r="D25" t="s">
-        <v>89</v>
-      </c>
-      <c r="E25" t="s">
-        <v>90</v>
-      </c>
-      <c r="F25" t="s">
-        <v>91</v>
-      </c>
       <c r="G25" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="H25" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="26" spans="1:11">
       <c r="A26">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" t="s">
+        <v>89</v>
+      </c>
+      <c r="E26" t="s">
+        <v>90</v>
+      </c>
+      <c r="F26" t="s">
+        <v>91</v>
+      </c>
+      <c r="G26" t="s">
         <v>92</v>
       </c>
-      <c r="C26" t="s">
-        <v>92</v>
-      </c>
-      <c r="D26" t="s">
-        <v>92</v>
-      </c>
-      <c r="E26" t="s">
+      <c r="H26" t="s">
+        <v>89</v>
+      </c>
+      <c r="I26" t="s">
         <v>93</v>
-      </c>
-      <c r="F26" t="s">
-        <v>94</v>
-      </c>
-      <c r="G26" t="s">
-        <v>95</v>
-      </c>
-      <c r="H26" t="s">
-        <v>92</v>
-      </c>
-      <c r="I26" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:11">
       <c r="A27">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B27" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" t="s">
+        <v>94</v>
+      </c>
+      <c r="D27" t="s">
+        <v>95</v>
+      </c>
+      <c r="E27" t="s">
+        <v>96</v>
+      </c>
+      <c r="F27" t="s">
         <v>97</v>
       </c>
-      <c r="C27" t="s">
-        <v>97</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="G27" t="s">
         <v>98</v>
       </c>
-      <c r="E27" t="s">
+      <c r="H27" t="s">
+        <v>94</v>
+      </c>
+      <c r="I27" t="s">
         <v>99</v>
-      </c>
-      <c r="F27" t="s">
-        <v>100</v>
-      </c>
-      <c r="G27" t="s">
-        <v>101</v>
-      </c>
-      <c r="H27" t="s">
-        <v>97</v>
-      </c>
-      <c r="I27" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:11">
       <c r="A28">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C28" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" t="s">
+        <v>197</v>
+      </c>
+      <c r="F28" t="s">
         <v>70</v>
       </c>
-      <c r="D28" t="s">
+      <c r="G28" t="s">
         <v>71</v>
       </c>
-      <c r="E28" t="s">
-        <v>200</v>
-      </c>
-      <c r="F28" t="s">
+      <c r="H28" t="s">
+        <v>72</v>
+      </c>
+      <c r="I28" t="s">
         <v>73</v>
       </c>
-      <c r="G28" t="s">
+      <c r="J28" t="s">
         <v>74</v>
-      </c>
-      <c r="H28" t="s">
-        <v>75</v>
-      </c>
-      <c r="I28" t="s">
-        <v>76</v>
-      </c>
-      <c r="J28" t="s">
-        <v>77</v>
       </c>
       <c r="K28">
         <v>2322071</v>
@@ -2105,95 +2105,95 @@
     </row>
     <row r="29" spans="1:11">
       <c r="A29">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B29" t="s">
+        <v>101</v>
+      </c>
+      <c r="C29" t="s">
+        <v>101</v>
+      </c>
+      <c r="D29" t="s">
+        <v>101</v>
+      </c>
+      <c r="E29" t="s">
+        <v>102</v>
+      </c>
+      <c r="F29" t="s">
+        <v>103</v>
+      </c>
+      <c r="G29" t="s">
         <v>104</v>
       </c>
-      <c r="C29" t="s">
-        <v>104</v>
-      </c>
-      <c r="D29" t="s">
-        <v>104</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="H29" t="s">
+        <v>101</v>
+      </c>
+      <c r="I29" t="s">
         <v>105</v>
       </c>
-      <c r="F29" t="s">
+      <c r="K29" t="s">
         <v>106</v>
-      </c>
-      <c r="G29" t="s">
-        <v>107</v>
-      </c>
-      <c r="H29" t="s">
-        <v>104</v>
-      </c>
-      <c r="I29" t="s">
-        <v>108</v>
-      </c>
-      <c r="K29" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:11">
       <c r="A30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B30" t="s">
+        <v>107</v>
+      </c>
+      <c r="C30" t="s">
+        <v>107</v>
+      </c>
+      <c r="D30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E30" t="s">
+        <v>108</v>
+      </c>
+      <c r="F30" t="s">
+        <v>109</v>
+      </c>
+      <c r="G30" t="s">
         <v>110</v>
       </c>
-      <c r="C30" t="s">
-        <v>110</v>
-      </c>
-      <c r="D30" t="s">
-        <v>110</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="H30" t="s">
+        <v>107</v>
+      </c>
+      <c r="J30" t="s">
         <v>111</v>
-      </c>
-      <c r="F30" t="s">
-        <v>112</v>
-      </c>
-      <c r="G30" t="s">
-        <v>113</v>
-      </c>
-      <c r="H30" t="s">
-        <v>110</v>
-      </c>
-      <c r="J30" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:11">
       <c r="A31">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C31" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D31" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E31" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F31" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="G31" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H31" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="I31" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="J31" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="K31">
         <v>2322084</v>
@@ -2201,34 +2201,34 @@
     </row>
     <row r="32" spans="1:11">
       <c r="A32">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B32" t="s">
+        <v>115</v>
+      </c>
+      <c r="C32" t="s">
+        <v>115</v>
+      </c>
+      <c r="D32" t="s">
+        <v>116</v>
+      </c>
+      <c r="E32" t="s">
+        <v>117</v>
+      </c>
+      <c r="F32" t="s">
         <v>118</v>
       </c>
-      <c r="C32" t="s">
-        <v>118</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="G32" t="s">
         <v>119</v>
       </c>
-      <c r="E32" t="s">
+      <c r="H32" t="s">
+        <v>115</v>
+      </c>
+      <c r="I32" t="s">
         <v>120</v>
       </c>
-      <c r="F32" t="s">
+      <c r="J32" t="s">
         <v>121</v>
-      </c>
-      <c r="G32" t="s">
-        <v>122</v>
-      </c>
-      <c r="H32" t="s">
-        <v>118</v>
-      </c>
-      <c r="I32" t="s">
-        <v>123</v>
-      </c>
-      <c r="J32" t="s">
-        <v>124</v>
       </c>
       <c r="K32">
         <v>2455145</v>
@@ -2236,34 +2236,34 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B33" t="s">
+        <v>201</v>
+      </c>
+      <c r="C33" t="s">
+        <v>201</v>
+      </c>
+      <c r="D33" t="s">
+        <v>201</v>
+      </c>
+      <c r="E33" t="s">
+        <v>202</v>
+      </c>
+      <c r="F33" t="s">
+        <v>203</v>
+      </c>
+      <c r="G33" t="s">
         <v>204</v>
       </c>
-      <c r="C33" t="s">
-        <v>204</v>
-      </c>
-      <c r="D33" t="s">
-        <v>204</v>
-      </c>
-      <c r="E33" t="s">
+      <c r="H33" t="s">
+        <v>201</v>
+      </c>
+      <c r="I33" t="s">
         <v>205</v>
       </c>
-      <c r="F33" t="s">
+      <c r="J33" t="s">
         <v>206</v>
-      </c>
-      <c r="G33" t="s">
-        <v>207</v>
-      </c>
-      <c r="H33" t="s">
-        <v>204</v>
-      </c>
-      <c r="I33" t="s">
-        <v>208</v>
-      </c>
-      <c r="J33" t="s">
-        <v>209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>